<commit_message>
actualizacion de combobox terminado
</commit_message>
<xml_diff>
--- a/Saves/ee.xlsx
+++ b/Saves/ee.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,17 +459,101 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1,2,3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Coord Diffusion</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Coord Absorption</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Coord Source</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Coord Mass</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Coord DamMass</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Coord CFlux</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Coord Convection</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Coord CSource</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[0]</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[0, 0]</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[0, 0]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[0, 0]</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>[0, 0]</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -484,7 +568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,14 +584,10 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>[55, 0, 0, 66]</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>[55, 66, 66, 88]</t>
-        </is>
-      </c>
+          <t>[45, 0, 0, 45]</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr"/>
       <c r="D1" t="inlineStr"/>
       <c r="E1" t="inlineStr"/>
       <c r="F1" t="inlineStr"/>
@@ -527,6 +607,7 @@
       <c r="T1" t="inlineStr"/>
       <c r="U1" t="inlineStr"/>
       <c r="V1" t="inlineStr"/>
+      <c r="W1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -551,6 +632,7 @@
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -575,6 +657,7 @@
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -599,6 +682,7 @@
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -623,6 +707,7 @@
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -647,6 +732,7 @@
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -671,6 +757,7 @@
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -695,6 +782,7 @@
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -719,6 +807,7 @@
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -743,6 +832,7 @@
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -767,6 +857,7 @@
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -791,6 +882,7 @@
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -815,6 +907,7 @@
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -839,6 +932,7 @@
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -863,6 +957,7 @@
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
@@ -887,6 +982,7 @@
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -911,6 +1007,7 @@
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
@@ -935,6 +1032,7 @@
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -959,6 +1057,7 @@
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
@@ -983,6 +1082,7 @@
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
@@ -1007,6 +1107,7 @@
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
@@ -1031,6 +1132,32 @@
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1043,14 +1170,598 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
+      <c r="F1" t="inlineStr"/>
+      <c r="G1" t="inlineStr"/>
+      <c r="H1" t="inlineStr"/>
+      <c r="I1" t="inlineStr"/>
+      <c r="J1" t="inlineStr"/>
+      <c r="K1" t="inlineStr"/>
+      <c r="L1" t="inlineStr"/>
+      <c r="M1" t="inlineStr"/>
+      <c r="N1" t="inlineStr"/>
+      <c r="O1" t="inlineStr"/>
+      <c r="P1" t="inlineStr"/>
+      <c r="Q1" t="inlineStr"/>
+      <c r="R1" t="inlineStr"/>
+      <c r="S1" t="inlineStr"/>
+      <c r="T1" t="inlineStr"/>
+      <c r="U1" t="inlineStr"/>
+      <c r="V1" t="inlineStr"/>
+      <c r="W1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1061,14 +1772,88 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>